<commit_message>
more cancel button fixed redireact cate to spec cate image delete not finish
</commit_message>
<xml_diff>
--- a/excel/04_17_2024.xlsx
+++ b/excel/04_17_2024.xlsx
@@ -13,6 +13,10 @@
     <sheet name="工作表04172024_154057" sheetId="4" state="visible" r:id="rId4"/>
     <sheet name="工作表04172024_155204" sheetId="5" state="visible" r:id="rId5"/>
     <sheet name="工作表04172024_155307" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="工作表04172024_161026" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="工作表04172024_161507" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="工作表04172024_161522" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="工作表04172024_161554" sheetId="10" state="visible" r:id="rId10"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -433,6 +437,113 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="25" customWidth="1" min="5" max="5"/>
+    <col width="25" customWidth="1" min="6" max="6"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>商品名稱</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>下單數量</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>售價</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>總價格</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>負責人</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>出單時間</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>789</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>56</v>
+      </c>
+      <c r="C2" t="n">
+        <v>789</v>
+      </c>
+      <c r="D2" t="n">
+        <v>44184</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>AnthonyFu</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>2024/04/17 07:53:05</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>傅垣幀</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>8</v>
+      </c>
+      <c r="C3" t="n">
+        <v>500</v>
+      </c>
+      <c r="D3" t="n">
+        <v>4000</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>AnthonyFu</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>2024/04/17 07:53:05</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
@@ -856,4 +967,325 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="25" customWidth="1" min="5" max="5"/>
+    <col width="25" customWidth="1" min="6" max="6"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>商品名稱</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>下單數量</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>售價</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>總價格</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>負責人</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>出單時間</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>789</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>56</v>
+      </c>
+      <c r="C2" t="n">
+        <v>789</v>
+      </c>
+      <c r="D2" t="n">
+        <v>44184</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>AnthonyFu</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>2024/04/17 07:53:05</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>傅垣幀</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>8</v>
+      </c>
+      <c r="C3" t="n">
+        <v>500</v>
+      </c>
+      <c r="D3" t="n">
+        <v>4000</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>AnthonyFu</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>2024/04/17 07:53:05</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="25" customWidth="1" min="5" max="5"/>
+    <col width="25" customWidth="1" min="6" max="6"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>商品名稱</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>下單數量</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>售價</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>總價格</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>負責人</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>出單時間</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>789</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>56</v>
+      </c>
+      <c r="C2" t="n">
+        <v>789</v>
+      </c>
+      <c r="D2" t="n">
+        <v>44184</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>AnthonyFu</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>2024/04/17 07:53:05</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>傅垣幀</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>8</v>
+      </c>
+      <c r="C3" t="n">
+        <v>500</v>
+      </c>
+      <c r="D3" t="n">
+        <v>4000</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>AnthonyFu</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>2024/04/17 07:53:05</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="25" customWidth="1" min="5" max="5"/>
+    <col width="25" customWidth="1" min="6" max="6"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>商品名稱</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>下單數量</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>售價</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>總價格</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>負責人</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>出單時間</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>789</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>56</v>
+      </c>
+      <c r="C2" t="n">
+        <v>789</v>
+      </c>
+      <c r="D2" t="n">
+        <v>44184</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>AnthonyFu</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>2024/04/17 07:53:05</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>傅垣幀</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>8</v>
+      </c>
+      <c r="C3" t="n">
+        <v>500</v>
+      </c>
+      <c r="D3" t="n">
+        <v>4000</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>AnthonyFu</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>2024/04/17 07:53:05</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>